<commit_message>
Attempts to use BEA etc data
</commit_message>
<xml_diff>
--- a/SAMdataPlus.xlsx
+++ b/SAMdataPlus.xlsx
@@ -1,30 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\GitFolders\CGE-Julia-EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1975DBB5-3D07-4333-B5FD-449D5E7E8C96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB5037F-73D8-4DBA-AAB3-09D6F87FC58A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12180" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1370" yWindow="1370" windowWidth="19180" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMdataPlus" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eli</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D8E61849-F3BB-42EA-B807-61839FAC0AFA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eli:"Converged to Infeasibility"</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Converged</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -144,29 +170,29 @@
     <t>Serv2-Sec6</t>
   </si>
   <si>
-    <t>Ag-Commod1</t>
-  </si>
-  <si>
-    <t>For-Commod2</t>
-  </si>
-  <si>
-    <t>Manf-Commod3</t>
-  </si>
-  <si>
-    <t>Manf2-Commod4</t>
-  </si>
-  <si>
-    <t>Serv-Commod5</t>
-  </si>
-  <si>
-    <t>Serv2-Commod6</t>
+    <t>Ag-Commod-1</t>
+  </si>
+  <si>
+    <t>For-Commod-2</t>
+  </si>
+  <si>
+    <t>Manf-Commod-3</t>
+  </si>
+  <si>
+    <t>Manf2-Commod-4</t>
+  </si>
+  <si>
+    <t>Serv-Commod-5</t>
+  </si>
+  <si>
+    <t>Serv2-Commod-6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +326,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1001,57 +1040,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="8.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>37</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" t="s">
-        <v>43</v>
       </c>
       <c r="N1" t="s">
         <v>8</v>
@@ -1143,20 +1186,41 @@
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>40</v>
-      </c>
-      <c r="I2">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>10</v>
+      </c>
+      <c r="T2">
+        <v>29</v>
+      </c>
+      <c r="Z2">
+        <v>3</v>
       </c>
       <c r="AA2">
         <v>5</v>
       </c>
       <c r="AB2">
         <f>SUM(B2:AA2)</f>
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="AC2">
         <v>1</v>
@@ -1183,8 +1247,8 @@
         <v>-2</v>
       </c>
       <c r="AK2">
-        <f>COUNTIF(A2:A29,"*commod*")</f>
-        <v>6</v>
+        <f>COUNTIF(A8:A29,"*commod*")</f>
+        <v>0</v>
       </c>
       <c r="AL2">
         <v>0.5</v>
@@ -1204,20 +1268,41 @@
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
         <v>2</v>
       </c>
-      <c r="H3">
-        <v>20</v>
-      </c>
-      <c r="I3">
+      <c r="J3" s="2">
+        <v>12</v>
+      </c>
+      <c r="K3" s="2">
+        <v>8</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5</v>
+      </c>
+      <c r="M3" s="2">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>10</v>
+      </c>
+      <c r="T3">
         <v>40</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
       </c>
       <c r="AA3">
         <v>5</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB27" si="0">SUM(B3:AA3)</f>
-        <v>65</v>
+        <f>SUM(B3:AA3)</f>
+        <v>92</v>
       </c>
       <c r="AC3">
         <v>1</v>
@@ -1246,21 +1331,41 @@
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>5</v>
+      </c>
+      <c r="L4" s="2">
         <v>3</v>
       </c>
-      <c r="J4">
-        <v>37</v>
-      </c>
-      <c r="K4">
-        <v>80</v>
-      </c>
-      <c r="P4" s="1"/>
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>30</v>
+      </c>
+      <c r="T4">
+        <v>140</v>
+      </c>
+      <c r="Z4">
+        <v>10</v>
+      </c>
       <c r="AA4">
         <v>16</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="0"/>
-        <v>133</v>
+        <f>SUM(B4:AA4)</f>
+        <v>219</v>
       </c>
       <c r="AC4">
         <v>1</v>
@@ -1289,21 +1394,41 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5">
-        <v>80</v>
-      </c>
-      <c r="K5">
-        <v>38</v>
-      </c>
-      <c r="P5" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+      <c r="J5" s="2">
+        <v>6</v>
+      </c>
+      <c r="K5" s="2">
+        <v>4</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>20</v>
+      </c>
+      <c r="T5">
+        <v>47</v>
+      </c>
+      <c r="Z5">
+        <v>5</v>
+      </c>
       <c r="AA5">
         <v>20</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="0"/>
-        <v>138</v>
+        <f>SUM(B5:AA5)</f>
+        <v>114</v>
       </c>
       <c r="AC5">
         <v>1</v>
@@ -1332,20 +1457,41 @@
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6">
-        <v>40</v>
-      </c>
-      <c r="M6">
+        <v>42</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
         <v>10</v>
+      </c>
+      <c r="K6" s="2">
+        <v>5</v>
+      </c>
+      <c r="L6" s="2">
+        <v>3</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>10</v>
+      </c>
+      <c r="T6">
+        <v>48</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
       </c>
       <c r="AA6">
         <v>15</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="0"/>
-        <v>65</v>
+        <f>SUM(B6:AA6)</f>
+        <v>98</v>
       </c>
       <c r="AC6">
         <v>1</v>
@@ -1374,20 +1520,41 @@
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7">
-        <v>13</v>
-      </c>
-      <c r="M7">
+        <v>43</v>
+      </c>
+      <c r="H7" s="2">
+        <v>3</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
         <v>40</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
       </c>
       <c r="AA7">
         <v>10</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="0"/>
-        <v>63</v>
+        <f>SUM(B7:AA7)</f>
+        <v>75</v>
       </c>
       <c r="AC7">
         <v>1</v>
@@ -1416,240 +1583,116 @@
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2">
-        <v>3</v>
-      </c>
-      <c r="S8">
-        <v>10</v>
-      </c>
-      <c r="T8">
-        <v>29</v>
-      </c>
-      <c r="Z8">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="0"/>
-        <v>72</v>
+        <f t="shared" ref="AB3:AB27" si="0">SUM(B8:AA8)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="S9">
-        <v>10</v>
-      </c>
-      <c r="T9">
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
         <v>40</v>
-      </c>
-      <c r="Z9">
-        <v>2</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
         <v>3</v>
       </c>
-      <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="S10">
-        <v>30</v>
-      </c>
-      <c r="T10">
-        <v>140</v>
-      </c>
-      <c r="Z10">
-        <v>10</v>
-      </c>
+      <c r="D10">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+      <c r="P10" s="1"/>
       <c r="AB10">
         <f t="shared" si="0"/>
-        <v>203</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="2">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2">
-        <v>3</v>
-      </c>
-      <c r="S11">
-        <v>20</v>
-      </c>
-      <c r="T11">
-        <v>47</v>
-      </c>
-      <c r="Z11">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>38</v>
+      </c>
+      <c r="P11" s="1"/>
       <c r="AB11">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2">
+        <v>36</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="G12">
         <v>10</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2</v>
-      </c>
-      <c r="S12">
-        <v>10</v>
-      </c>
-      <c r="T12">
-        <v>48</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
       </c>
       <c r="AB12">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="2">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2">
-        <v>3</v>
-      </c>
-      <c r="S13">
-        <v>5</v>
-      </c>
-      <c r="T13">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
         <v>40</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
       </c>
       <c r="AB13">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="H14" s="2">
         <v>29</v>
       </c>
-      <c r="C14" s="2">
+      <c r="I14" s="2">
         <v>30</v>
       </c>
-      <c r="D14" s="2">
+      <c r="J14" s="2">
         <v>120</v>
       </c>
-      <c r="E14" s="2">
+      <c r="K14" s="2">
         <v>50</v>
       </c>
-      <c r="F14" s="2">
+      <c r="L14" s="2">
         <v>40</v>
       </c>
-      <c r="G14" s="2">
+      <c r="M14" s="2">
         <v>33</v>
       </c>
       <c r="AB14">
@@ -1661,22 +1704,22 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2">
+      <c r="H15" s="2">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="I15" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="2">
+      <c r="J15" s="2">
         <v>16</v>
       </c>
-      <c r="E15" s="2">
+      <c r="K15" s="2">
         <v>20</v>
       </c>
-      <c r="F15" s="2">
+      <c r="L15" s="2">
         <v>15</v>
       </c>
-      <c r="G15" s="2">
+      <c r="M15" s="2">
         <v>10</v>
       </c>
       <c r="AB15">
@@ -1688,22 +1731,22 @@
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
+      <c r="H16" s="2">
         <v>8</v>
       </c>
-      <c r="C16" s="2">
+      <c r="I16" s="2">
         <v>8</v>
       </c>
-      <c r="D16" s="2">
+      <c r="J16" s="2">
         <v>15</v>
       </c>
-      <c r="E16" s="2">
+      <c r="K16" s="2">
         <v>20</v>
       </c>
-      <c r="F16" s="2">
+      <c r="L16" s="2">
         <v>12</v>
       </c>
-      <c r="G16" s="2">
+      <c r="M16" s="2">
         <v>8</v>
       </c>
       <c r="AB16">
@@ -1715,22 +1758,22 @@
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17">
+      <c r="H17">
         <v>30</v>
       </c>
-      <c r="C17">
+      <c r="I17">
         <v>30</v>
       </c>
-      <c r="D17">
+      <c r="J17">
         <v>20</v>
       </c>
-      <c r="E17">
+      <c r="K17">
         <v>30</v>
       </c>
-      <c r="F17">
+      <c r="L17">
         <v>18</v>
       </c>
-      <c r="G17">
+      <c r="M17">
         <v>22</v>
       </c>
       <c r="R17" s="1"/>
@@ -1746,22 +1789,22 @@
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B18">
+      <c r="H18">
         <v>10</v>
       </c>
-      <c r="C18">
+      <c r="I18">
         <v>10</v>
       </c>
-      <c r="D18">
+      <c r="J18">
         <v>50</v>
       </c>
-      <c r="E18">
+      <c r="K18">
         <v>40</v>
       </c>
-      <c r="F18">
+      <c r="L18">
         <v>16</v>
       </c>
-      <c r="G18">
+      <c r="M18">
         <v>14</v>
       </c>
       <c r="S18">
@@ -1777,23 +1820,23 @@
         <v>4</v>
       </c>
       <c r="U19">
-        <f>SUM(B21:T21)</f>
+        <f>SUM(H21:T21)</f>
         <v>38</v>
       </c>
       <c r="V19">
-        <f>SUM(B22:T22)</f>
+        <f>SUM(H22:T22)</f>
         <v>56</v>
       </c>
       <c r="W19">
-        <f>SUM(H23:T23)</f>
+        <f>SUM(B23:T23)</f>
         <v>42</v>
       </c>
       <c r="X19">
-        <f>SUM(B24:T24)</f>
+        <f>SUM(H24:T24)</f>
         <v>144</v>
       </c>
       <c r="Y19">
-        <f>SUM(H25:T25)</f>
+        <f>SUM(B25:T25)</f>
         <v>23</v>
       </c>
       <c r="AB19">
@@ -1806,11 +1849,11 @@
         <v>5</v>
       </c>
       <c r="Q20">
-        <f>SUM(B17:S17)</f>
+        <f>SUM(H17:S17)</f>
         <v>210</v>
       </c>
       <c r="R20">
-        <f>SUM(B18:S18)</f>
+        <f>SUM(H18:S18)</f>
         <v>260</v>
       </c>
       <c r="S20">
@@ -1825,22 +1868,22 @@
       <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B21">
+      <c r="H21">
         <v>6</v>
       </c>
-      <c r="C21">
+      <c r="I21">
         <v>6</v>
       </c>
-      <c r="D21">
+      <c r="J21">
         <v>4</v>
       </c>
-      <c r="E21">
+      <c r="K21">
         <v>6</v>
       </c>
-      <c r="F21">
+      <c r="L21">
         <v>8</v>
       </c>
-      <c r="G21">
+      <c r="M21">
         <v>8</v>
       </c>
       <c r="S21">
@@ -1855,22 +1898,22 @@
       <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B22">
+      <c r="H22">
         <v>4</v>
       </c>
-      <c r="C22">
+      <c r="I22">
         <v>4</v>
       </c>
-      <c r="D22">
+      <c r="J22">
         <v>16</v>
       </c>
-      <c r="E22">
+      <c r="K22">
         <v>20</v>
       </c>
-      <c r="F22">
+      <c r="L22">
         <v>6</v>
       </c>
-      <c r="G22">
+      <c r="M22">
         <v>6</v>
       </c>
       <c r="S22">
@@ -1885,22 +1928,22 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="H23">
+      <c r="B23">
         <v>4</v>
       </c>
-      <c r="I23">
+      <c r="C23">
         <v>6</v>
       </c>
-      <c r="J23">
+      <c r="D23">
         <v>12</v>
       </c>
-      <c r="K23">
+      <c r="E23">
         <v>5</v>
       </c>
-      <c r="L23">
+      <c r="F23">
         <v>8</v>
       </c>
-      <c r="M23">
+      <c r="G23">
         <v>7</v>
       </c>
       <c r="S23">
@@ -1927,22 +1970,22 @@
       <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="H25">
+      <c r="B25">
         <v>4</v>
       </c>
-      <c r="I25">
+      <c r="C25">
         <v>4</v>
       </c>
-      <c r="J25">
+      <c r="D25">
         <v>6</v>
       </c>
-      <c r="K25">
+      <c r="E25">
         <v>4</v>
       </c>
-      <c r="L25">
+      <c r="F25">
         <v>3</v>
       </c>
-      <c r="M25">
+      <c r="G25">
         <v>2</v>
       </c>
       <c r="AB25">
@@ -1958,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <f>SUM(Z8:Z13)</f>
+        <f>SUM(Z2:Z7)</f>
         <v>20</v>
       </c>
       <c r="AA26">
@@ -1973,26 +2016,26 @@
       <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="H27">
+      <c r="B27">
         <v>8</v>
       </c>
-      <c r="I27">
+      <c r="C27">
         <v>8</v>
       </c>
-      <c r="J27">
+      <c r="D27">
         <v>12</v>
       </c>
-      <c r="K27">
+      <c r="E27">
         <v>23</v>
       </c>
-      <c r="L27">
+      <c r="F27">
         <v>10</v>
       </c>
-      <c r="M27">
+      <c r="G27">
         <v>10</v>
       </c>
       <c r="AB27">
-        <f>SUM(B27:AA27)</f>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
@@ -2001,53 +2044,53 @@
         <v>18</v>
       </c>
       <c r="B28">
-        <f>SUM(B2:B27)</f>
+        <f t="shared" ref="B28:AA28" si="1">SUM(B2:B27)</f>
+        <v>76</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
         <v>109</v>
       </c>
-      <c r="C28">
-        <f t="shared" ref="C28:AA28" si="1">SUM(C2:C27)</f>
+      <c r="I28">
+        <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="D28">
+      <c r="J28">
         <f t="shared" si="1"/>
         <v>289</v>
       </c>
-      <c r="E28">
+      <c r="K28">
         <f t="shared" si="1"/>
         <v>223</v>
       </c>
-      <c r="F28">
+      <c r="L28">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="G28">
+      <c r="M28">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="1"/>
-        <v>147</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
       <c r="N28">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2101,7 +2144,7 @@
         <v>20</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="1"/>
+        <f>SUM(AA2:AA27)</f>
         <v>71</v>
       </c>
       <c r="AB28">
@@ -2113,9 +2156,9 @@
       <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="M29">
-        <f>SUM(B28:M28)-SUM(AB2:AB13)</f>
-        <v>444</v>
+      <c r="G29">
+        <f>SUM(B28:G28)-SUM(AB2:AB7)</f>
+        <v>-81</v>
       </c>
       <c r="P29">
         <f>SUM(N28:P28)-SUM(AB14:AB16)</f>
@@ -2168,5 +2211,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>